<commit_message>
Added neatfast and vallado to repository. Updated code to load/save after each phase, fixed plotting bugs, and probably other bug fixes.
</commit_message>
<xml_diff>
--- a/config/config_tests.xlsx
+++ b/config/config_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2194b9ba31d909a4/Documents/Classes/Research/neat-mt/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="769" documentId="8_{556BF41C-AE9B-443F-857D-8B96428591C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4CEC195C-D8B3-4D14-B758-6B4E7001444D}"/>
+  <xr:revisionPtr revIDLastSave="825" documentId="8_{556BF41C-AE9B-443F-857D-8B96428591C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{B2137D52-28F4-48D5-A0FF-F49E494D3019}"/>
   <bookViews>
-    <workbookView xWindow="-11745" yWindow="4410" windowWidth="23145" windowHeight="14610" activeTab="1" xr2:uid="{8FD9BE4C-F606-4879-908F-EE57D8FAFC01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8FD9BE4C-F606-4879-908F-EE57D8FAFC01}"/>
   </bookViews>
   <sheets>
     <sheet name="NEAT Parameters" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="197">
   <si>
     <t>Parameter</t>
   </si>
@@ -252,9 +252,6 @@
     <t>Same as 9 but lower compatibility threshold to allow more than one species. Took maybe a third longer (35 sec/gen vs 25 sec/gen because it started with around 20 species). Overall pretty solid performance, but it would be nice to have slightly better runtime.</t>
   </si>
   <si>
-    <t>Same as 10  but with 500 population to see if the difference in performance is notable. Final performance was the same, but anecdotally, the thrust history on this run seemed a little less refined than run 10. That could be due to different runs and if run several times, a "smooth" control may appear. Overall, approximately same performance for around a quarter the time.</t>
-  </si>
-  <si>
     <t>max_generations</t>
   </si>
   <si>
@@ -447,9 +444,6 @@
     <t>Fitness Function Run #</t>
   </si>
   <si>
-    <t>Adjusted the way that the fitnesses are normalized when performing roulette wheel selection - previously it grossly over-preferenced the top performers. Also adjusted the missed thrust cases for use with fitness function tuning. This had many cases reach "Performing close capture" but couldn't improve past a certain point. This is a good benchmark set of parameters for fitness function tuning.</t>
-  </si>
-  <si>
     <t>This was the set of fitness function parameters that I had been using previously. This had many cases reach "Performing close capture" but couldn't improve past a certain point. This is a good benchmark set of NEAT parameters for fitness function tuning.</t>
   </si>
   <si>
@@ -601,6 +595,36 @@
   </si>
   <si>
     <t>Increased max energy and decreased min energy to give the network more room to work, but also increased big_penalty for going outside energy bounds. No noticable difference - maybe a slight improvement? Probably doesn't matter, but I'll keep the change.</t>
+  </si>
+  <si>
+    <t>NOTE: In the context of training a network in two phases, coarse and fine, where the second phase does include missed thrust and needs all the inputs, the first phase will need all the inputs as well. While the above settings are fine for a fixed trajectory, this can't be used for a network that will ultimately be trained for missed thrust.</t>
+  </si>
+  <si>
+    <t>33 but with 5 hidden nodes and fitness function 17. Did ok - not necessarily better than 3 hidden nodes.</t>
+  </si>
+  <si>
+    <t>Tried with 4 hidden nodes instead of 5. Again, did ok but not necessarily better than 3.</t>
+  </si>
+  <si>
+    <t>Stagnation at 133</t>
+  </si>
+  <si>
+    <t>Went straight to lots of missed thrust. Not super great.</t>
+  </si>
+  <si>
+    <t>Stagnation at 175</t>
+  </si>
+  <si>
+    <t>This should be a good benchmark set for fitness function tuning</t>
+  </si>
+  <si>
+    <t>Adjusted the way that the fitnesses are normalized when performing roulette wheel selection - previously it way over-preferenced the top performers. Also adjusted the missed thrust cases for use with fitness function tuning. This had many cases reach "Performing close capture" but couldn't improve past a certain point.</t>
+  </si>
+  <si>
+    <t>Changed population to 500 to see if the difference in performance is notable. Final performance was the same, but the thrust history on this run seemed a little less refined than run 10. That could be due to different runs and if run several times, a "smooth" control may appear. Overall, approximately same performance for around a quarter the time.</t>
+  </si>
+  <si>
+    <t>Trying lots of missed thrust with 3 hidden nodes. Did about the same as with 4 hidden nodes. Potentially suggests that either: 1. two phases are needed and the current settings are meant for phase 1, and/or 2. these settings are not good for a single run</t>
   </si>
 </sst>
 </file>
@@ -638,12 +662,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -667,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -701,6 +737,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1019,18 +1070,13 @@
   <dimension ref="A1:BI60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AK47" sqref="AK47"/>
+      <pane xSplit="1" topLeftCell="AL1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AP47" sqref="AP47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="35.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="11" width="34" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.42578125" style="1" customWidth="1"/>
-    <col min="13" max="37" width="34" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="35.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1133,7 +1179,7 @@
       <c r="AG1" s="3">
         <v>32</v>
       </c>
-      <c r="AH1" s="3">
+      <c r="AH1" s="12">
         <v>33</v>
       </c>
       <c r="AI1" s="3">
@@ -1318,7 +1364,7 @@
       <c r="AG2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="AH2" s="7" t="s">
+      <c r="AH2" s="13" t="s">
         <v>54</v>
       </c>
       <c r="AI2" s="7" t="s">
@@ -1330,6 +1376,9 @@
       <c r="AK2" s="7" t="s">
         <v>54</v>
       </c>
+      <c r="AL2" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1431,7 +1480,7 @@
       <c r="AG3" s="1">
         <v>500</v>
       </c>
-      <c r="AH3" s="1">
+      <c r="AH3" s="14">
         <v>500</v>
       </c>
       <c r="AI3" s="1">
@@ -1443,10 +1492,13 @@
       <c r="AK3" s="1">
         <v>500</v>
       </c>
+      <c r="AL3" s="1">
+        <v>500</v>
+      </c>
     </row>
     <row r="4" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="1">
         <v>200</v>
@@ -1544,7 +1596,7 @@
       <c r="AG4" s="1">
         <v>200</v>
       </c>
-      <c r="AH4" s="1">
+      <c r="AH4" s="14">
         <v>200</v>
       </c>
       <c r="AI4" s="1">
@@ -1554,6 +1606,9 @@
         <v>200</v>
       </c>
       <c r="AK4" s="1">
+        <v>200</v>
+      </c>
+      <c r="AL4" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1657,7 +1712,7 @@
       <c r="AG5" s="1">
         <v>0</v>
       </c>
-      <c r="AH5" s="1">
+      <c r="AH5" s="14">
         <v>0</v>
       </c>
       <c r="AI5" s="1">
@@ -1667,6 +1722,9 @@
         <v>0</v>
       </c>
       <c r="AK5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1770,7 +1828,7 @@
       <c r="AG6" s="1">
         <v>1</v>
       </c>
-      <c r="AH6" s="1">
+      <c r="AH6" s="14">
         <v>1</v>
       </c>
       <c r="AI6" s="1">
@@ -1781,6 +1839,12 @@
       </c>
       <c r="AK6" s="1">
         <v>1</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN6" s="1">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.25">
@@ -1883,7 +1947,7 @@
       <c r="AG7" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="AH7" s="1" t="b">
+      <c r="AH7" s="14" t="b">
         <v>1</v>
       </c>
       <c r="AI7" s="1" t="b">
@@ -1893,6 +1957,9 @@
         <v>1</v>
       </c>
       <c r="AK7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL7" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1996,7 +2063,7 @@
       <c r="AG8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="AH8" s="1" t="b">
+      <c r="AH8" s="14" t="b">
         <v>0</v>
       </c>
       <c r="AI8" s="1" t="b">
@@ -2007,6 +2074,12 @@
       </c>
       <c r="AK8" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="AL8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:61" x14ac:dyDescent="0.25">
@@ -2109,7 +2182,7 @@
       <c r="AG9" s="1">
         <v>1</v>
       </c>
-      <c r="AH9" s="1">
+      <c r="AH9" s="14">
         <v>1</v>
       </c>
       <c r="AI9" s="1">
@@ -2119,6 +2192,9 @@
         <v>1</v>
       </c>
       <c r="AK9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL9" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2222,7 +2298,7 @@
       <c r="AG10" s="1">
         <v>1</v>
       </c>
-      <c r="AH10" s="1">
+      <c r="AH10" s="14">
         <v>1</v>
       </c>
       <c r="AI10" s="1">
@@ -2232,6 +2308,9 @@
         <v>1</v>
       </c>
       <c r="AK10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL10" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2335,7 +2414,7 @@
       <c r="AG11" s="1">
         <v>7</v>
       </c>
-      <c r="AH11" s="1">
+      <c r="AH11" s="14">
         <v>7</v>
       </c>
       <c r="AI11" s="1">
@@ -2346,6 +2425,9 @@
       </c>
       <c r="AK11" s="1">
         <v>2</v>
+      </c>
+      <c r="AL11" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:61" x14ac:dyDescent="0.25">
@@ -2448,7 +2530,7 @@
       <c r="AG12" s="1">
         <v>3</v>
       </c>
-      <c r="AH12" s="1">
+      <c r="AH12" s="14">
         <v>3</v>
       </c>
       <c r="AI12" s="1">
@@ -2459,6 +2541,15 @@
       </c>
       <c r="AK12" s="1">
         <v>5</v>
+      </c>
+      <c r="AL12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AO12" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:61" x14ac:dyDescent="0.25">
@@ -2561,7 +2652,7 @@
       <c r="AG13" s="1">
         <v>2</v>
       </c>
-      <c r="AH13" s="1">
+      <c r="AH13" s="14">
         <v>2</v>
       </c>
       <c r="AI13" s="1">
@@ -2571,6 +2662,9 @@
         <v>2</v>
       </c>
       <c r="AK13" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL13" s="1">
         <v>2</v>
       </c>
     </row>
@@ -2674,7 +2768,7 @@
       <c r="AG14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AH14" s="1" t="s">
+      <c r="AH14" s="14" t="s">
         <v>69</v>
       </c>
       <c r="AI14" s="1" t="s">
@@ -2684,6 +2778,9 @@
         <v>69</v>
       </c>
       <c r="AK14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL14" s="1" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2787,7 +2884,7 @@
       <c r="AG15" s="1">
         <v>1</v>
       </c>
-      <c r="AH15" s="1">
+      <c r="AH15" s="14">
         <v>1</v>
       </c>
       <c r="AI15" s="1">
@@ -2797,6 +2894,9 @@
         <v>1</v>
       </c>
       <c r="AK15" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL15" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2900,7 +3000,7 @@
       <c r="AG16" s="1">
         <v>0.6</v>
       </c>
-      <c r="AH16" s="1">
+      <c r="AH16" s="14">
         <v>0.6</v>
       </c>
       <c r="AI16" s="1">
@@ -2912,8 +3012,11 @@
       <c r="AK16" s="1">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL16" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -3013,7 +3116,7 @@
       <c r="AG17" s="1">
         <v>0.05</v>
       </c>
-      <c r="AH17" s="1">
+      <c r="AH17" s="14">
         <v>0.05</v>
       </c>
       <c r="AI17" s="1">
@@ -3025,8 +3128,11 @@
       <c r="AK17" s="1">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL17" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
@@ -3126,7 +3232,7 @@
       <c r="AG18" s="1">
         <v>0.05</v>
       </c>
-      <c r="AH18" s="1">
+      <c r="AH18" s="14">
         <v>0.05</v>
       </c>
       <c r="AI18" s="1">
@@ -3138,8 +3244,11 @@
       <c r="AK18" s="1">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL18" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
@@ -3239,7 +3348,7 @@
       <c r="AG19" s="1">
         <v>0.05</v>
       </c>
-      <c r="AH19" s="1">
+      <c r="AH19" s="14">
         <v>0.05</v>
       </c>
       <c r="AI19" s="1">
@@ -3251,8 +3360,11 @@
       <c r="AK19" s="1">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL19" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
@@ -3352,7 +3464,7 @@
       <c r="AG20" s="1">
         <v>0.05</v>
       </c>
-      <c r="AH20" s="1">
+      <c r="AH20" s="14">
         <v>0.05</v>
       </c>
       <c r="AI20" s="1">
@@ -3364,8 +3476,11 @@
       <c r="AK20" s="1">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL20" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>17</v>
       </c>
@@ -3465,7 +3580,7 @@
       <c r="AG21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AH21" s="1" t="s">
+      <c r="AH21" s="14" t="s">
         <v>55</v>
       </c>
       <c r="AI21" s="1" t="s">
@@ -3477,8 +3592,11 @@
       <c r="AK21" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL21" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>19</v>
       </c>
@@ -3578,7 +3696,7 @@
       <c r="AG22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AH22" s="1" t="s">
+      <c r="AH22" s="14" t="s">
         <v>20</v>
       </c>
       <c r="AI22" s="1" t="s">
@@ -3590,8 +3708,11 @@
       <c r="AK22" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
@@ -3691,7 +3812,7 @@
       <c r="AG23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AH23" s="1" t="s">
+      <c r="AH23" s="14" t="s">
         <v>56</v>
       </c>
       <c r="AI23" s="1" t="s">
@@ -3703,8 +3824,11 @@
       <c r="AK23" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL23" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
@@ -3804,7 +3928,7 @@
       <c r="AG24" s="1">
         <v>1E-3</v>
       </c>
-      <c r="AH24" s="1">
+      <c r="AH24" s="14">
         <v>1E-3</v>
       </c>
       <c r="AI24" s="1">
@@ -3816,8 +3940,11 @@
       <c r="AK24" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL24" s="1">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
@@ -3917,7 +4044,7 @@
       <c r="AG25" s="1">
         <v>1.5</v>
       </c>
-      <c r="AH25" s="1">
+      <c r="AH25" s="14">
         <v>1.5</v>
       </c>
       <c r="AI25" s="1">
@@ -3929,8 +4056,11 @@
       <c r="AK25" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL25" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>27</v>
       </c>
@@ -4030,7 +4160,7 @@
       <c r="AG26" s="1">
         <v>0.4</v>
       </c>
-      <c r="AH26" s="1">
+      <c r="AH26" s="14">
         <v>0.4</v>
       </c>
       <c r="AI26" s="1">
@@ -4042,8 +4172,11 @@
       <c r="AK26" s="1">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL26" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -4143,7 +4276,7 @@
       <c r="AG27" s="1">
         <v>0.4</v>
       </c>
-      <c r="AH27" s="1">
+      <c r="AH27" s="14">
         <v>0.4</v>
       </c>
       <c r="AI27" s="1">
@@ -4155,8 +4288,11 @@
       <c r="AK27" s="1">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL27" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -4256,7 +4392,7 @@
       <c r="AG28" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AH28" s="1">
+      <c r="AH28" s="14">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AI28" s="1">
@@ -4268,8 +4404,11 @@
       <c r="AK28" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL28" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
@@ -4369,7 +4508,7 @@
       <c r="AG29" s="1">
         <v>0.05</v>
       </c>
-      <c r="AH29" s="1">
+      <c r="AH29" s="14">
         <v>0.05</v>
       </c>
       <c r="AI29" s="1">
@@ -4381,8 +4520,11 @@
       <c r="AK29" s="1">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL29" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
@@ -4482,7 +4624,7 @@
       <c r="AG30" s="1">
         <v>1.5</v>
       </c>
-      <c r="AH30" s="1">
+      <c r="AH30" s="14">
         <v>1.5</v>
       </c>
       <c r="AI30" s="1">
@@ -4494,8 +4636,11 @@
       <c r="AK30" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL30" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
@@ -4595,7 +4740,7 @@
       <c r="AG31" s="1">
         <v>0.1</v>
       </c>
-      <c r="AH31" s="1">
+      <c r="AH31" s="14">
         <v>0.1</v>
       </c>
       <c r="AI31" s="1">
@@ -4607,8 +4752,11 @@
       <c r="AK31" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL31" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
@@ -4708,7 +4856,7 @@
       <c r="AG32" s="1">
         <v>0.4</v>
       </c>
-      <c r="AH32" s="1">
+      <c r="AH32" s="14">
         <v>0.4</v>
       </c>
       <c r="AI32" s="1">
@@ -4720,8 +4868,11 @@
       <c r="AK32" s="1">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL32" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>34</v>
       </c>
@@ -4821,7 +4972,7 @@
       <c r="AG33" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AH33" s="1">
+      <c r="AH33" s="14">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AI33" s="1">
@@ -4833,8 +4984,11 @@
       <c r="AK33" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL33" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
@@ -4934,7 +5088,7 @@
       <c r="AG34" s="1">
         <v>0.2</v>
       </c>
-      <c r="AH34" s="1">
+      <c r="AH34" s="14">
         <v>0.2</v>
       </c>
       <c r="AI34" s="1">
@@ -4946,8 +5100,11 @@
       <c r="AK34" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL34" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>36</v>
       </c>
@@ -5047,7 +5204,7 @@
       <c r="AG35" s="1">
         <v>0</v>
       </c>
-      <c r="AH35" s="1">
+      <c r="AH35" s="14">
         <v>0</v>
       </c>
       <c r="AI35" s="1">
@@ -5059,8 +5216,11 @@
       <c r="AK35" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
@@ -5160,7 +5320,7 @@
       <c r="AG36" s="1">
         <v>3.33</v>
       </c>
-      <c r="AH36" s="1">
+      <c r="AH36" s="14">
         <v>3.33</v>
       </c>
       <c r="AI36" s="1">
@@ -5172,8 +5332,11 @@
       <c r="AK36" s="1">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL36" s="1">
+        <v>3.33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>38</v>
       </c>
@@ -5273,7 +5436,7 @@
       <c r="AG37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AH37" s="1" t="s">
+      <c r="AH37" s="14" t="s">
         <v>39</v>
       </c>
       <c r="AI37" s="1" t="s">
@@ -5285,8 +5448,11 @@
       <c r="AK37" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL37" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>40</v>
       </c>
@@ -5386,7 +5552,7 @@
       <c r="AG38" s="1">
         <v>50</v>
       </c>
-      <c r="AH38" s="1">
+      <c r="AH38" s="14">
         <v>50</v>
       </c>
       <c r="AI38" s="1">
@@ -5398,8 +5564,11 @@
       <c r="AK38" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL38" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>41</v>
       </c>
@@ -5499,7 +5668,7 @@
       <c r="AG39" s="1">
         <v>1</v>
       </c>
-      <c r="AH39" s="1">
+      <c r="AH39" s="14">
         <v>1</v>
       </c>
       <c r="AI39" s="1">
@@ -5511,8 +5680,11 @@
       <c r="AK39" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>42</v>
       </c>
@@ -5612,7 +5784,7 @@
       <c r="AG40" s="1">
         <v>0.5</v>
       </c>
-      <c r="AH40" s="1">
+      <c r="AH40" s="14">
         <v>0.6</v>
       </c>
       <c r="AI40" s="1">
@@ -5624,10 +5796,13 @@
       <c r="AK40" s="1">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL40" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
@@ -5725,7 +5900,7 @@
       <c r="AG41" s="1">
         <v>10</v>
       </c>
-      <c r="AH41" s="1">
+      <c r="AH41" s="14">
         <v>10</v>
       </c>
       <c r="AI41" s="1">
@@ -5737,10 +5912,13 @@
       <c r="AK41" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL41" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
@@ -5838,7 +6016,7 @@
       <c r="AG42" s="1">
         <v>4</v>
       </c>
-      <c r="AH42" s="1">
+      <c r="AH42" s="14">
         <v>4</v>
       </c>
       <c r="AI42" s="1">
@@ -5850,11 +6028,15 @@
       <c r="AK42" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL42" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
-    </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AH43" s="14"/>
+    </row>
+    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>45</v>
       </c>
@@ -5931,7 +6113,7 @@
         <v>-11.03</v>
       </c>
       <c r="Z44" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA44" s="1">
         <v>-62.2</v>
@@ -5943,7 +6125,7 @@
         <v>-98.1</v>
       </c>
       <c r="AD44" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AE44" s="1">
         <v>-74</v>
@@ -5954,20 +6136,32 @@
       <c r="AG44" s="1">
         <v>-56</v>
       </c>
-      <c r="AH44" s="1">
+      <c r="AH44" s="14">
         <v>-57.5</v>
       </c>
       <c r="AI44" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AJ44" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AK44" s="1">
         <v>-0.87</v>
       </c>
-    </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL44" s="1">
+        <v>-0.94</v>
+      </c>
+      <c r="AM44" s="1">
+        <v>-0.95</v>
+      </c>
+      <c r="AN44" s="1">
+        <v>-248.67</v>
+      </c>
+      <c r="AO44" s="1">
+        <v>-213.81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>57</v>
       </c>
@@ -6056,7 +6250,7 @@
         <v>359.2</v>
       </c>
       <c r="AD45" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AE45" s="1">
         <v>355.7</v>
@@ -6067,20 +6261,32 @@
       <c r="AG45" s="1">
         <v>118.6</v>
       </c>
-      <c r="AH45" s="1">
+      <c r="AH45" s="14">
         <v>121</v>
       </c>
       <c r="AI45" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AJ45" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AK45" s="1">
         <v>120.1</v>
       </c>
-    </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL45" s="1">
+        <v>153.4</v>
+      </c>
+      <c r="AM45" s="1">
+        <v>148.5</v>
+      </c>
+      <c r="AN45" s="1">
+        <v>1443.4</v>
+      </c>
+      <c r="AO45" s="1">
+        <v>1887.3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>48</v>
       </c>
@@ -6121,7 +6327,7 @@
         <v>49</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O46" s="1" t="s">
         <v>49</v>
@@ -6133,7 +6339,7 @@
         <v>49</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S46" s="1" t="s">
         <v>49</v>
@@ -6145,7 +6351,7 @@
         <v>49</v>
       </c>
       <c r="V46" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W46" s="1" t="s">
         <v>49</v>
@@ -6169,7 +6375,7 @@
         <v>49</v>
       </c>
       <c r="AD46" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AE46" s="1" t="s">
         <v>49</v>
@@ -6180,11 +6386,11 @@
       <c r="AG46" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AH46" s="1" t="s">
+      <c r="AH46" s="14" t="s">
         <v>49</v>
       </c>
       <c r="AI46" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AJ46" s="1" t="s">
         <v>49</v>
@@ -6192,8 +6398,20 @@
       <c r="AK46" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="47" spans="1:37" s="5" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="AL46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN46" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AO46" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="47" spans="1:41" s="5" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>43</v>
       </c>
@@ -6228,85 +6446,97 @@
         <v>71</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>72</v>
+        <v>195</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P47" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q47" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="Q47" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="R47" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="S47" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="S47" s="5" t="s">
+      <c r="T47" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="T47" s="5" t="s">
+      <c r="U47" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="U47" s="5" t="s">
+      <c r="V47" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="V47" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="W47" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="X47" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="X47" s="5" t="s">
+      <c r="Y47" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="Y47" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="Z47" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AA47" s="5" t="s">
-        <v>137</v>
+        <v>194</v>
       </c>
       <c r="AB47" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AC47" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AD47" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="AE47" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF47" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="AE47" s="5" t="s">
+      <c r="AG47" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="AF47" s="5" t="s">
+      <c r="AH47" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="AG47" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="AH47" s="5" t="s">
-        <v>155</v>
-      </c>
       <c r="AI47" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="AJ47" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="AK47" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="AK47" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL47" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="AM47" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="AN47" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="AO47" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -6317,7 +6547,7 @@
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -6328,62 +6558,86 @@
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA50" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="AK50" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AA51" s="16"/>
+      <c r="AK51" s="16"/>
+    </row>
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AA52" s="16"/>
+      <c r="AK52" s="16"/>
+    </row>
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AA53" s="16"/>
+      <c r="AK53" s="16"/>
+    </row>
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AA54" s="16"/>
+      <c r="AK54" s="16"/>
+    </row>
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA55" s="16"/>
+      <c r="AK55" s="16"/>
+    </row>
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="AK56" s="16"/>
+    </row>
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="AK57" s="16"/>
+    </row>
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AK58" s="16"/>
+    </row>
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK59" s="16"/>
+    </row>
+    <row r="60" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="AK50:AK59"/>
+    <mergeCell ref="AA50:AA55"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6396,7 +6650,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S21" sqref="S21"/>
+      <selection pane="topRight" activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6502,167 +6756,167 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B10" s="1">
         <v>100</v>
@@ -6688,7 +6942,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" s="1">
         <v>50</v>
@@ -6709,27 +6963,27 @@
         <v>100</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K11" s="1">
         <v>50</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" s="1">
         <v>10</v>
@@ -6755,7 +7009,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B13" s="1">
         <v>5</v>
@@ -6764,107 +7018,107 @@
         <v>5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B14" s="1">
         <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B18" s="1" t="b">
         <v>1</v>
@@ -6884,7 +7138,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B19" s="1">
         <v>10000</v>
@@ -6907,7 +7161,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20" s="1" t="b">
         <v>1</v>
@@ -6927,7 +7181,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
@@ -6947,7 +7201,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B22" s="1">
         <v>1000</v>
@@ -6967,73 +7221,73 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="C25" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B27" s="1">
         <v>26</v>
@@ -7163,7 +7417,7 @@
         <v>137</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N30" s="1">
         <v>116.2</v>
@@ -7201,10 +7455,10 @@
         <v>49</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>49</v>
@@ -7225,7 +7479,7 @@
         <v>49</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>49</v>
@@ -7242,55 +7496,55 @@
         <v>43</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>140</v>
-      </c>
       <c r="D33" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>145</v>
-      </c>
       <c r="F33" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I33" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="J33" s="5" t="s">
-        <v>166</v>
-      </c>
       <c r="K33" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="L33" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="L33" s="5" t="s">
-        <v>169</v>
-      </c>
       <c r="M33" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="N33" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="N33" s="5" t="s">
-        <v>174</v>
-      </c>
       <c r="O33" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="P33" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="Q33" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="R33" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="R33" s="5" t="s">
-        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>